<commit_message>
Actualizacion del plan general del proyecto
</commit_message>
<xml_diff>
--- a/tspi/ciclo-3/plan3-20105914.xlsx
+++ b/tspi/ciclo-3/plan3-20105914.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecvasro\workspace\github\PPR\tspi\ciclo-3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="33520" windowHeight="20540" tabRatio="400" activeTab="1"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="33525" windowHeight="20535" tabRatio="400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
     <sheet name="task" sheetId="2" r:id="rId2"/>
     <sheet name="logt" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Id</t>
   </si>
@@ -160,6 +165,9 @@
   <si>
     <t>Terminar de definir estrategia de desarrollo</t>
   </si>
+  <si>
+    <t>Conociendo el funcionamiento de redmine e importer.</t>
+  </si>
 </sst>
 </file>
 
@@ -266,7 +274,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -330,9 +338,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -723,19 +728,19 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="7" customWidth="1"/>
     <col min="3" max="4" width="46" style="7" customWidth="1"/>
-    <col min="5" max="6" width="15.6640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="2.5" style="6" customWidth="1"/>
-    <col min="8" max="12" width="15.6640625" style="6" customWidth="1"/>
-    <col min="13" max="1013" width="11.5" style="6"/>
-    <col min="1014" max="16384" width="11.5" style="5"/>
+    <col min="5" max="6" width="15.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="2.42578125" style="6" customWidth="1"/>
+    <col min="8" max="12" width="15.7109375" style="6" customWidth="1"/>
+    <col min="13" max="1013" width="11.42578125" style="6"/>
+    <col min="1014" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1013" s="3" customFormat="1" ht="26">
+    <row r="1" spans="1:1013" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1013" ht="36">
+    <row r="2" spans="1:1013" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>46</v>
       </c>
@@ -1808,7 +1813,7 @@
       <c r="ALX2" s="4"/>
       <c r="ALY2" s="4"/>
     </row>
-    <row r="3" spans="1:1013" ht="48">
+    <row r="3" spans="1:1013" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>47</v>
       </c>
@@ -2845,7 +2850,7 @@
       <c r="ALX3" s="4"/>
       <c r="ALY3" s="4"/>
     </row>
-    <row r="4" spans="1:1013">
+    <row r="4" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>53</v>
       </c>
@@ -3882,7 +3887,7 @@
       <c r="ALX4" s="4"/>
       <c r="ALY4" s="4"/>
     </row>
-    <row r="5" spans="1:1013" ht="24">
+    <row r="5" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>55</v>
       </c>
@@ -4919,7 +4924,7 @@
       <c r="ALX5" s="4"/>
       <c r="ALY5" s="4"/>
     </row>
-    <row r="6" spans="1:1013" ht="24">
+    <row r="6" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>57</v>
       </c>
@@ -5956,7 +5961,7 @@
       <c r="ALX6" s="4"/>
       <c r="ALY6" s="4"/>
     </row>
-    <row r="7" spans="1:1013" ht="24">
+    <row r="7" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>58</v>
       </c>
@@ -6993,7 +6998,7 @@
       <c r="ALX7" s="4"/>
       <c r="ALY7" s="4"/>
     </row>
-    <row r="8" spans="1:1013" ht="24">
+    <row r="8" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>61</v>
       </c>
@@ -8030,7 +8035,7 @@
       <c r="ALX8" s="4"/>
       <c r="ALY8" s="4"/>
     </row>
-    <row r="9" spans="1:1013" ht="24">
+    <row r="9" spans="1:1013" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>63</v>
       </c>
@@ -8065,7 +8070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:1013">
+    <row r="10" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>65</v>
       </c>
@@ -8100,7 +8105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:1013" ht="36">
+    <row r="11" spans="1:1013" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>66</v>
       </c>
@@ -8135,7 +8140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1013">
+    <row r="12" spans="1:1013" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -8168,16 +8173,16 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.5" style="5"/>
+    <col min="1" max="1" width="3.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30.75" customHeight="1">
+    <row r="1" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8188,7 +8193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>46</v>
       </c>
@@ -8200,7 +8205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>47</v>
       </c>
@@ -8212,98 +8217,108 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4">
         <f>SUMIF(logt!$G:$G,A4,logt!$F:$F)/60</f>
-        <v>4</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C4" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="12" customFormat="1">
-      <c r="A5" s="31">
-        <v>58</v>
+    <row r="5" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>57</v>
       </c>
       <c r="B5" s="4">
         <f>SUMIF(logt!$G:$G,A5,logt!$F:$F)/60</f>
-        <v>1.5</v>
-      </c>
-      <c r="C5" s="31">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="4">
-        <v>61</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="30">
+        <v>58</v>
       </c>
       <c r="B6" s="4">
         <f>SUMIF(logt!$G:$G,A6,logt!$F:$F)/60</f>
         <v>1.5</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="30">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>61</v>
+      </c>
+      <c r="B7" s="4">
+        <f>SUMIF(logt!$G:$G,A7,logt!$F:$F)/60</f>
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" s="12" customFormat="1">
-      <c r="A8" s="31"/>
+    <row r="8" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="30"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
   </sheetData>
+  <sortState ref="A2:C7">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -8323,22 +8338,22 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A9" sqref="A9:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="21" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="21" customWidth="1"/>
+    <col min="3" max="4" width="13.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="11.83203125" style="5"/>
+    <col min="9" max="16384" width="11.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" ht="26">
+    <row r="1" spans="1:8" s="13" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>13</v>
       </c>
@@ -8364,7 +8379,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="23">
         <v>41938</v>
       </c>
@@ -8387,11 +8402,11 @@
       <c r="G2" s="21">
         <v>46</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>41938</v>
       </c>
@@ -8414,16 +8429,16 @@
       <c r="G3" s="21">
         <v>47</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>41942</v>
       </c>
       <c r="B4" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="14">
         <v>0.91666666666666663</v>
@@ -8441,11 +8456,11 @@
       <c r="G4" s="21">
         <v>61</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="27">
         <v>41943</v>
       </c>
@@ -8472,7 +8487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <v>41944</v>
       </c>
@@ -8499,7 +8514,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="24">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>41944</v>
       </c>
@@ -8516,7 +8531,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="15">
-        <f t="shared" ref="F7" si="1">((HOUR(D7)-HOUR(C7))*60)+(MINUTE(D7)-MINUTE(C7))-E7</f>
+        <f t="shared" ref="F7:F9" si="1">((HOUR(D7)-HOUR(C7))*60)+(MINUTE(D7)-MINUTE(C7))-E7</f>
         <v>240</v>
       </c>
       <c r="G7" s="4">
@@ -8526,40 +8541,75 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="22"/>
-      <c r="H8" s="9"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
+        <v>41943</v>
+      </c>
+      <c r="B8" s="22">
+        <v>6</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.65486111111111112</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="G8" s="21">
+        <v>53</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="28"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="18"/>
-      <c r="H9" s="9"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
+        <v>41920</v>
+      </c>
+      <c r="B9" s="21">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0.875</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.97361111111111109</v>
+      </c>
+      <c r="E9" s="21">
+        <v>12</v>
+      </c>
+      <c r="F9" s="18">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="28"/>
-      <c r="B10" s="30"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="22"/>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="28"/>
-      <c r="B11" s="30"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="22"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="22"/>
       <c r="C12" s="17"/>
@@ -8567,7 +8617,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="22"/>
       <c r="C13" s="17"/>
@@ -8575,7 +8625,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="22"/>
       <c r="C14" s="17"/>
@@ -8583,7 +8633,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="22"/>
       <c r="C15" s="17"/>
@@ -8591,7 +8641,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="18" spans="1:8" s="12" customFormat="1">
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="24"/>
       <c r="B18" s="26"/>
       <c r="C18" s="25"/>
@@ -8601,7 +8651,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="22"/>
       <c r="C19" s="17"/>
@@ -8609,7 +8659,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="18"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="22"/>
       <c r="C20" s="17"/>
@@ -8617,7 +8667,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="22"/>
       <c r="C21" s="17"/>
@@ -8625,7 +8675,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="22"/>
       <c r="C22" s="17"/>
@@ -8633,7 +8683,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="22"/>
       <c r="C23" s="17"/>
@@ -8641,7 +8691,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="22"/>
       <c r="C24" s="17"/>
@@ -8649,7 +8699,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="22"/>
       <c r="C25" s="17"/>
@@ -8657,7 +8707,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="18"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="22"/>
       <c r="C26" s="17"/>
@@ -8665,7 +8715,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="18"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="22"/>
       <c r="C27" s="17"/>
@@ -8673,7 +8723,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="22"/>
       <c r="C28" s="17"/>
@@ -8681,7 +8731,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="18"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="22"/>
       <c r="C29" s="17"/>
@@ -8689,7 +8739,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="18"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="22"/>
       <c r="C30" s="17"/>
@@ -8697,7 +8747,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="22"/>
       <c r="C31" s="17"/>
@@ -8705,7 +8755,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="18"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="22"/>
       <c r="C32" s="17"/>
@@ -8713,7 +8763,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="22"/>
       <c r="C33" s="17"/>
@@ -8721,7 +8771,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="18"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="22"/>
       <c r="C34" s="17"/>

</xml_diff>